<commit_message>
21.03 various images and graphs
</commit_message>
<xml_diff>
--- a/experimental-setup/11.03 growth-curve protocol.xlsx
+++ b/experimental-setup/11.03 growth-curve protocol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\64204\Desktop\master\experimental-setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7D854C-9303-40D9-8539-68CC4BF079D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CB9094-E840-411E-86F3-08D74B285647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E388B108-E347-41DE-9585-A2159611B410}"/>
+    <workbookView xWindow="5985" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{E388B108-E347-41DE-9585-A2159611B410}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
   <si>
     <t>A</t>
   </si>
@@ -147,6 +147,51 @@
   </si>
   <si>
     <t>17.03 First screen with PAO1</t>
+  </si>
+  <si>
+    <t>23.03 GFP (or eGFP) only!</t>
+  </si>
+  <si>
+    <t>445 LESB</t>
+  </si>
+  <si>
+    <t>446 LESB</t>
+  </si>
+  <si>
+    <t>317 PAO1</t>
+  </si>
+  <si>
+    <t>318 PAO1</t>
+  </si>
+  <si>
+    <t>366 PAO1</t>
+  </si>
+  <si>
+    <t>367 PAO1</t>
+  </si>
+  <si>
+    <t>308 PAO1</t>
+  </si>
+  <si>
+    <t>309 PAO1</t>
+  </si>
+  <si>
+    <t>323 PA14</t>
+  </si>
+  <si>
+    <t>324 PA14</t>
+  </si>
+  <si>
+    <t>3 PAO1</t>
+  </si>
+  <si>
+    <t>4 LESB</t>
+  </si>
+  <si>
+    <t>6 PA14</t>
+  </si>
+  <si>
+    <t>23.03 Actual setup: LESB grew too slowly</t>
   </si>
 </sst>
 </file>
@@ -162,7 +207,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,6 +256,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -341,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -358,8 +415,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -368,7 +424,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -377,12 +433,29 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08F8FC58-50B5-42B1-B80F-083BEDBB2893}">
-  <dimension ref="A1:AA11"/>
+  <dimension ref="A1:AA21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="78" workbookViewId="0">
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,22 +908,22 @@
       <c r="O4" t="s">
         <v>0</v>
       </c>
-      <c r="P4" s="18" t="s">
+      <c r="P4" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="20"/>
-      <c r="V4" s="27" t="s">
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="W4" s="28"/>
-      <c r="X4" s="28"/>
-      <c r="Y4" s="28"/>
-      <c r="Z4" s="28"/>
-      <c r="AA4" s="29"/>
+      <c r="W4" s="27"/>
+      <c r="X4" s="27"/>
+      <c r="Y4" s="27"/>
+      <c r="Z4" s="27"/>
+      <c r="AA4" s="28"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -867,22 +940,22 @@
       <c r="O5" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="21" t="s">
+      <c r="P5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="22"/>
-      <c r="V5" s="30" t="s">
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="W5" s="26"/>
-      <c r="X5" s="26"/>
-      <c r="Y5" s="26"/>
-      <c r="Z5" s="26"/>
-      <c r="AA5" s="31"/>
+      <c r="W5" s="25"/>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="25"/>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="30"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -907,22 +980,22 @@
       <c r="O6" t="s">
         <v>2</v>
       </c>
-      <c r="P6" s="21" t="s">
+      <c r="P6" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="22"/>
-      <c r="V6" s="30" t="s">
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="21"/>
+      <c r="V6" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="W6" s="26"/>
-      <c r="X6" s="26"/>
-      <c r="Y6" s="26"/>
-      <c r="Z6" s="26"/>
-      <c r="AA6" s="31"/>
+      <c r="W6" s="25"/>
+      <c r="X6" s="25"/>
+      <c r="Y6" s="25"/>
+      <c r="Z6" s="25"/>
+      <c r="AA6" s="30"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -931,22 +1004,22 @@
       <c r="O7" t="s">
         <v>3</v>
       </c>
-      <c r="P7" s="23" t="s">
+      <c r="P7" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
-      <c r="S7" s="24"/>
-      <c r="T7" s="24"/>
-      <c r="U7" s="25"/>
-      <c r="V7" s="32" t="s">
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="24"/>
+      <c r="V7" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="W7" s="33"/>
-      <c r="X7" s="33"/>
-      <c r="Y7" s="33"/>
-      <c r="Z7" s="33"/>
-      <c r="AA7" s="34"/>
+      <c r="W7" s="32"/>
+      <c r="X7" s="32"/>
+      <c r="Y7" s="32"/>
+      <c r="Z7" s="32"/>
+      <c r="AA7" s="33"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -971,20 +1044,14 @@
       <c r="O8" t="s">
         <v>4</v>
       </c>
-      <c r="P8" s="18" t="s">
+      <c r="P8" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="20"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="16"/>
-      <c r="X8" s="16"/>
-      <c r="Y8" s="16"/>
-      <c r="Z8" s="16"/>
-      <c r="AA8" s="16"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="19"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1001,20 +1068,14 @@
       <c r="O9" t="s">
         <v>5</v>
       </c>
-      <c r="P9" s="21" t="s">
+      <c r="P9" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="22"/>
-      <c r="V9" s="16"/>
-      <c r="W9" s="16"/>
-      <c r="X9" s="16"/>
-      <c r="Y9" s="16"/>
-      <c r="Z9" s="16"/>
-      <c r="AA9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="21"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1039,22 +1100,22 @@
       <c r="O10" t="s">
         <v>6</v>
       </c>
-      <c r="P10" s="21" t="s">
+      <c r="P10" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="22"/>
-      <c r="V10" s="35" t="s">
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="21"/>
+      <c r="V10" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="W10" s="36"/>
-      <c r="X10" s="36"/>
-      <c r="Y10" s="36"/>
-      <c r="Z10" s="36"/>
-      <c r="AA10" s="37"/>
+      <c r="W10" s="35"/>
+      <c r="X10" s="35"/>
+      <c r="Y10" s="35"/>
+      <c r="Z10" s="35"/>
+      <c r="AA10" s="36"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1079,22 +1140,390 @@
       <c r="O11" t="s">
         <v>7</v>
       </c>
-      <c r="P11" s="23" t="s">
+      <c r="P11" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="24"/>
-      <c r="U11" s="25"/>
-      <c r="V11" s="38" t="s">
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="W11" s="39"/>
-      <c r="X11" s="39"/>
-      <c r="Y11" s="39"/>
-      <c r="Z11" s="39"/>
-      <c r="AA11" s="40"/>
+      <c r="W11" s="38"/>
+      <c r="X11" s="38"/>
+      <c r="Y11" s="38"/>
+      <c r="Z11" s="38"/>
+      <c r="AA11" s="39"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="O12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>6</v>
+      </c>
+      <c r="H13">
+        <v>7</v>
+      </c>
+      <c r="I13">
+        <v>8</v>
+      </c>
+      <c r="J13">
+        <v>9</v>
+      </c>
+      <c r="K13">
+        <v>10</v>
+      </c>
+      <c r="L13">
+        <v>11</v>
+      </c>
+      <c r="M13">
+        <v>12</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>2</v>
+      </c>
+      <c r="R13">
+        <v>3</v>
+      </c>
+      <c r="S13">
+        <v>4</v>
+      </c>
+      <c r="T13">
+        <v>5</v>
+      </c>
+      <c r="U13">
+        <v>6</v>
+      </c>
+      <c r="V13">
+        <v>7</v>
+      </c>
+      <c r="W13">
+        <v>8</v>
+      </c>
+      <c r="X13">
+        <v>9</v>
+      </c>
+      <c r="Y13">
+        <v>10</v>
+      </c>
+      <c r="Z13">
+        <v>11</v>
+      </c>
+      <c r="AA13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="46"/>
+      <c r="O14" t="s">
+        <v>0</v>
+      </c>
+      <c r="P14" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="18"/>
+      <c r="T14" s="18"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="W14" s="54"/>
+      <c r="X14" s="54"/>
+      <c r="Y14" s="54"/>
+      <c r="Z14" s="54"/>
+      <c r="AA14" s="55"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="48"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="48"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="49"/>
+      <c r="O15" t="s">
+        <v>1</v>
+      </c>
+      <c r="P15" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q15" s="56"/>
+      <c r="R15" s="56"/>
+      <c r="S15" s="56"/>
+      <c r="T15" s="56"/>
+      <c r="U15" s="21"/>
+      <c r="V15" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="W15" s="54"/>
+      <c r="X15" s="54"/>
+      <c r="Y15" s="54"/>
+      <c r="Z15" s="54"/>
+      <c r="AA15" s="55"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="46"/>
+      <c r="O16" t="s">
+        <v>2</v>
+      </c>
+      <c r="P16" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q16" s="56"/>
+      <c r="R16" s="56"/>
+      <c r="S16" s="56"/>
+      <c r="T16" s="56"/>
+      <c r="U16" s="21"/>
+      <c r="V16" s="53"/>
+      <c r="W16" s="53"/>
+      <c r="X16" s="53"/>
+      <c r="Y16" s="53"/>
+      <c r="Z16" s="53"/>
+      <c r="AA16" s="53"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="43"/>
+      <c r="O17" t="s">
+        <v>3</v>
+      </c>
+      <c r="P17" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="24"/>
+      <c r="V17" s="53"/>
+      <c r="W17" s="53"/>
+      <c r="X17" s="53"/>
+      <c r="Y17" s="53"/>
+      <c r="Z17" s="53"/>
+      <c r="AA17" s="53"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="41"/>
+      <c r="O18" t="s">
+        <v>4</v>
+      </c>
+      <c r="P18" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="18"/>
+      <c r="T18" s="18"/>
+      <c r="U18" s="19"/>
+      <c r="V18" s="53"/>
+      <c r="W18" s="53"/>
+      <c r="X18" s="53"/>
+      <c r="Y18" s="53"/>
+      <c r="Z18" s="53"/>
+      <c r="AA18" s="53"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="41"/>
+      <c r="O19" t="s">
+        <v>5</v>
+      </c>
+      <c r="P19" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
+      <c r="U19" s="24"/>
+      <c r="V19" s="53"/>
+      <c r="W19" s="53"/>
+      <c r="X19" s="53"/>
+      <c r="Y19" s="53"/>
+      <c r="Z19" s="53"/>
+      <c r="AA19" s="53"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="52"/>
+      <c r="O20" t="s">
+        <v>6</v>
+      </c>
+      <c r="P20" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="18"/>
+      <c r="T20" s="18"/>
+      <c r="U20" s="19"/>
+      <c r="V20" s="53"/>
+      <c r="W20" s="53"/>
+      <c r="X20" s="53"/>
+      <c r="Y20" s="53"/>
+      <c r="Z20" s="53"/>
+      <c r="AA20" s="53"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="49"/>
+      <c r="O21" t="s">
+        <v>7</v>
+      </c>
+      <c r="P21" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="W21" s="54"/>
+      <c r="X21" s="54"/>
+      <c r="Y21" s="54"/>
+      <c r="Z21" s="54"/>
+      <c r="AA21" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>